<commit_message>
arquitectura inicial, fuentes y estilos bases
</commit_message>
<xml_diff>
--- a/ANOTACIONES MOBILE DESIGN.xlsx
+++ b/ANOTACIONES MOBILE DESIGN.xlsx
@@ -9,11 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="figma" sheetId="1" r:id="rId1"/>
     <sheet name="arquitectura inicial" sheetId="2" r:id="rId2"/>
+    <sheet name="fuentes" sheetId="3" r:id="rId3"/>
+    <sheet name="estilos bases" sheetId="4" r:id="rId4"/>
+    <sheet name="header" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,16 +28,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>HERAMIENTO DE DISEÑADORES</t>
   </si>
+  <si>
+    <t>ojo solo deben ser 2 tipos de fuentes</t>
+  </si>
+  <si>
+    <t>dm sans</t>
+  </si>
+  <si>
+    <t>google fonts</t>
+  </si>
+  <si>
+    <t>copiamos este link y lo pegamos debajo de title</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -42,13 +57,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -63,8 +92,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -114,6 +144,685 @@
         <a:xfrm>
           <a:off x="0" y="38100"/>
           <a:ext cx="3781425" cy="2991267"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>553370</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>181567</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4629150" y="1276350"/>
+          <a:ext cx="6592220" cy="4239217"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>55524</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>75286</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="13009524" cy="7314286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Elipse 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="123825" y="2847975"/>
+          <a:ext cx="2714625" cy="857250"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-AR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Elipse 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2933700" y="2828924"/>
+          <a:ext cx="7248525" cy="3400425"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-AR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Elipse 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10477500" y="2276475"/>
+          <a:ext cx="2714625" cy="857250"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-AR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>65049</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>103861</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9525" y="409575"/>
+          <a:ext cx="13009524" cy="7314286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>171451</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Elipse 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="3600451"/>
+          <a:ext cx="2838450" cy="1095374"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-AR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Elipse 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5876925" y="4648201"/>
+          <a:ext cx="2838450" cy="1095374"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-AR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Elipse 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11010900" y="4638675"/>
+          <a:ext cx="1600200" cy="514350"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-AR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>55524</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>189586</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="8305800"/>
+          <a:ext cx="13009524" cy="7314286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>851</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>532</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagen 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="15811500"/>
+          <a:ext cx="6096851" cy="3810532"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>144244</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>162198</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagen 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6334125" y="18211800"/>
+          <a:ext cx="9812119" cy="1952898"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>219930</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>29440</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9334500" y="114300"/>
+          <a:ext cx="6125430" cy="6201640"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>115592</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>824</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9259592" cy="5906324"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -411,7 +1120,74 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="D25" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I95"/>
+  <sheetViews>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="H105" sqref="H105"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D43" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I95" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
se agregaron estilos al header, h1, p y boton - header completado
</commit_message>
<xml_diff>
--- a/ANOTACIONES MOBILE DESIGN.xlsx
+++ b/ANOTACIONES MOBILE DESIGN.xlsx
@@ -9,16 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="5" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="figma" sheetId="1" r:id="rId1"/>
     <sheet name="arquitectura inicial" sheetId="2" r:id="rId2"/>
     <sheet name="fuentes" sheetId="3" r:id="rId3"/>
-    <sheet name="estilos bases" sheetId="4" r:id="rId4"/>
-    <sheet name="header" sheetId="5" r:id="rId5"/>
-    <sheet name="clases bem header" sheetId="6" r:id="rId6"/>
-    <sheet name="estil backraound h1" sheetId="7" r:id="rId7"/>
+    <sheet name="Hoja1" sheetId="8" r:id="rId4"/>
+    <sheet name="estilos bases" sheetId="4" r:id="rId5"/>
+    <sheet name="header" sheetId="5" r:id="rId6"/>
+    <sheet name="clases bem header" sheetId="6" r:id="rId7"/>
+    <sheet name="estil backraound h1" sheetId="7" r:id="rId8"/>
+    <sheet name="boton position flotante" sheetId="9" r:id="rId9"/>
+    <sheet name="secc intercambio" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>HERAMIENTO DE DISEÑADORES</t>
   </si>
@@ -55,12 +58,27 @@
   <si>
     <t>Uso de linear-gradient</t>
   </si>
+  <si>
+    <t>https://www.figma.com/file/sMmlQaZldfDcLERYYWe6h4/Bata-Bit?node-id=83%3A132</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nota importante; si quieremos buscar un archivo de una carpeta a otra utilizar; </t>
+  </si>
+  <si>
+    <t>../</t>
+  </si>
+  <si>
+    <t>Uso de position para botón flotante</t>
+  </si>
+  <si>
+    <t>Estructura base de la sección de intercambio</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,6 +105,19 @@
       <b/>
       <sz val="24"/>
       <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -117,11 +148,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -450,15 +485,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>65049</xdr:colOff>
+      <xdr:colOff>74574</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>103861</xdr:rowOff>
+      <xdr:rowOff>151486</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -475,7 +510,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9525" y="409575"/>
+          <a:off x="19050" y="457200"/>
           <a:ext cx="13009524" cy="7314286"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1121,6 +1156,206 @@
         <a:xfrm>
           <a:off x="6858000" y="190500"/>
           <a:ext cx="7363853" cy="5449060"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>581957</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>86029</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="685800"/>
+          <a:ext cx="6677957" cy="2181529"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>257743</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>67110</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6858000" y="685800"/>
+          <a:ext cx="4067743" cy="3115110"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>390897</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>342974</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7629525" y="0"/>
+          <a:ext cx="2667372" cy="533474"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>819</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>9763</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="228600" y="4972050"/>
+          <a:ext cx="5868219" cy="1705213"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>505955</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>76728</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="28575" y="866775"/>
+          <a:ext cx="8097380" cy="3781953"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1414,6 +1649,41 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:M1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
@@ -1431,21 +1701,30 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I95"/>
+  <dimension ref="A1:M95"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="H105" sqref="H105"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
+      <c r="G1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
     </row>
     <row r="43" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D43" s="1" t="s">
@@ -1468,7 +1747,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1479,7 +1770,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K9"/>
   <sheetViews>
@@ -1506,7 +1797,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1521,12 +1812,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1548,5 +1839,47 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:K3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="K2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
se incia confecion del main y estilos
</commit_message>
<xml_diff>
--- a/ANOTACIONES MOBILE DESIGN.xlsx
+++ b/ANOTACIONES MOBILE DESIGN.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="5" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="figma" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="clases bem header" sheetId="6" r:id="rId7"/>
     <sheet name="estil backraound h1" sheetId="7" r:id="rId8"/>
     <sheet name="boton position flotante" sheetId="9" r:id="rId9"/>
-    <sheet name="secc intercambio" sheetId="10" r:id="rId10"/>
+    <sheet name="secc intercambio main" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -71,7 +71,7 @@
     <t>Uso de position para botón flotante</t>
   </si>
   <si>
-    <t>Estructura base de la sección de intercambio</t>
+    <t>Estructura base de la sección de intercambio MAIN</t>
   </si>
 </sst>
 </file>
@@ -152,10 +152,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1356,6 +1356,87 @@
         <a:xfrm>
           <a:off x="28575" y="866775"/>
           <a:ext cx="8097380" cy="3781953"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>715645</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>67083</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="862853"/>
+          <a:ext cx="9097645" cy="2924583"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>381479</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>105375</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9144000" y="862853"/>
+          <a:ext cx="3429479" cy="4296375"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1654,7 +1735,7 @@
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1681,6 +1762,7 @@
     <mergeCell ref="A1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1716,15 +1798,15 @@
       <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
     </row>
     <row r="43" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D43" s="1" t="s">
@@ -1823,16 +1905,16 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1854,17 +1936,17 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
       <c r="K2" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
agregado imagen de backround bitcoin, estilos de h2 y p
</commit_message>
<xml_diff>
--- a/ANOTACIONES MOBILE DESIGN.xlsx
+++ b/ANOTACIONES MOBILE DESIGN.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="6" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="8" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="figma" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,8 @@
     <sheet name="estil backraound h1" sheetId="7" r:id="rId8"/>
     <sheet name="boton position flotante" sheetId="9" r:id="rId9"/>
     <sheet name="secc intercambio main" sheetId="10" r:id="rId10"/>
+    <sheet name="img backround h2" sheetId="11" r:id="rId11"/>
+    <sheet name="tablas" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -246,6 +248,308 @@
         <a:xfrm>
           <a:off x="4629150" y="1276350"/>
           <a:ext cx="6592220" cy="4239217"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>734272</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>172192</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="6068272" cy="5315692"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Elipse 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2124075" y="2695574"/>
+          <a:ext cx="1819275" cy="1476375"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-AR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Conector recto de flecha 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3800475" y="2990850"/>
+          <a:ext cx="2914650" cy="76200"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>353112</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>9766</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6858000" y="2857500"/>
+          <a:ext cx="4925112" cy="1724266"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>496119</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>28899</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagen 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6819900" y="2847975"/>
+          <a:ext cx="5868219" cy="2324424"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>409951</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>171660</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagen 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="5715000"/>
+          <a:ext cx="2695951" cy="1505160"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>209898</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>85950</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagen 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3048000" y="5715000"/>
+          <a:ext cx="2495898" cy="1609950"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1734,7 +2038,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
@@ -1763,6 +2067,35 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1929,7 +2262,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
se le dieron estilos a las tablas
</commit_message>
<xml_diff>
--- a/ANOTACIONES MOBILE DESIGN.xlsx
+++ b/ANOTACIONES MOBILE DESIGN.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="7" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="8" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="figma" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,8 @@
     <sheet name="secc intercambio main" sheetId="10" r:id="rId9"/>
     <sheet name="img backround h2" sheetId="11" r:id="rId10"/>
     <sheet name="tablas" sheetId="12" r:id="rId11"/>
+    <sheet name="estilo tablas" sheetId="13" r:id="rId12"/>
+    <sheet name="deta estil tabl moneda" sheetId="14" r:id="rId13"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -166,14 +168,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -660,6 +662,244 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>553272</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>19771</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2476500"/>
+          <a:ext cx="5887272" cy="5163271"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>353006</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>38743</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="4163006" cy="4610743"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>610111</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>85976</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4572000" y="190500"/>
+          <a:ext cx="3658111" cy="1800476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>534219</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>77035</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="5868219" cy="5982535"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>343586</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>134166</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6096000" y="0"/>
+          <a:ext cx="4915586" cy="5849166"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>686959</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>124560</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="6286500"/>
+          <a:ext cx="8306959" cy="5268060"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2128,7 +2368,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2165,14 +2405,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="4" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="5" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2180,6 +2420,36 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="N37" sqref="N37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2215,7 +2485,7 @@
       <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H1" s="3"/>
@@ -2313,16 +2583,16 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2344,17 +2614,17 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
       <c r="K2" t="s">
         <v>9</v>
       </c>
@@ -2385,21 +2655,21 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
finalizo estilos de la tabla 1
</commit_message>
<xml_diff>
--- a/ANOTACIONES MOBILE DESIGN.xlsx
+++ b/ANOTACIONES MOBILE DESIGN.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="8" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="9" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="figma" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="tablas" sheetId="12" r:id="rId11"/>
     <sheet name="estilo tablas" sheetId="13" r:id="rId12"/>
     <sheet name="deta estil tabl moneda" sheetId="14" r:id="rId13"/>
+    <sheet name="secc beneficios" sheetId="15" r:id="rId14"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -894,6 +895,44 @@
         <a:xfrm>
           <a:off x="0" y="6286500"/>
           <a:ext cx="8306959" cy="5268060"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>295742</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>143294</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9144000" y="6096000"/>
+          <a:ext cx="3343742" cy="3000794"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2442,14 +2481,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="N37" sqref="N37"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="N51" sqref="N51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
llegue hasta la foto de la espelucada
</commit_message>
<xml_diff>
--- a/ANOTACIONES MOBILE DESIGN.xlsx
+++ b/ANOTACIONES MOBILE DESIGN.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="9" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="9" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="figma" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,10 @@
     <sheet name="tablas" sheetId="12" r:id="rId11"/>
     <sheet name="estilo tablas" sheetId="13" r:id="rId12"/>
     <sheet name="deta estil tabl moneda" sheetId="14" r:id="rId13"/>
-    <sheet name="secc beneficios" sheetId="15" r:id="rId14"/>
+    <sheet name="estrucutu beneficios" sheetId="15" r:id="rId14"/>
+    <sheet name="tarjetas secc beneficios" sheetId="16" r:id="rId15"/>
+    <sheet name="comodin foto grande" sheetId="17" r:id="rId16"/>
+    <sheet name="secc planes" sheetId="18" r:id="rId17"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -933,6 +936,854 @@
         <a:xfrm>
           <a:off x="9144000" y="6096000"/>
           <a:ext cx="3343742" cy="3000794"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>19489</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>57633</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9067800" y="9553575"/>
+          <a:ext cx="3143689" cy="3458058"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>581411</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>19257</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Imagen 10"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8486775" y="57150"/>
+          <a:ext cx="2762636" cy="1486107"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>39275</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>48004</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="190500"/>
+          <a:ext cx="8421275" cy="2715004"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="969689" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="CuadroTexto 3"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11582400" y="381000"/>
+          <a:ext cx="969689" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100"/>
+            <a:t>arriba</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100" baseline="0"/>
+            <a:t> y abajo</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-AR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1313501" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="CuadroTexto 4"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11372850" y="904875"/>
+          <a:ext cx="1313501" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100"/>
+            <a:t>derecha e izquierda</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>132280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Conector recto de flecha 6"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="9705975" y="513280"/>
+          <a:ext cx="1876425" cy="486845"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>685801</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Conector recto de flecha 7"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="10191750" y="962025"/>
+          <a:ext cx="1162051" cy="85725"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>66874</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Imagen 15"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="3209925"/>
+          <a:ext cx="6848475" cy="1428949"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>67421</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>171717</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Imagen 16"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6915150" y="3400425"/>
+          <a:ext cx="5344271" cy="1914792"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1925079" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="CuadroTexto 17"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6353175" y="3438525"/>
+          <a:ext cx="1925079" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100"/>
+            <a:t>posicionar el loguito de batata</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>552837</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>76883</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Imagen 18"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="66675" y="5276850"/>
+          <a:ext cx="2772162" cy="4896533"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>743798</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>162320</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Imagen 19"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6096000" y="6286500"/>
+          <a:ext cx="6077798" cy="2829320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>486906</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>134007</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="190500"/>
+          <a:ext cx="8106906" cy="4706007"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>343480</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>143666</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8382000" y="190500"/>
+          <a:ext cx="4153480" cy="5668166"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>733425</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>200908</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>382</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8353425" y="4695825"/>
+          <a:ext cx="6325483" cy="2734057"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>667375</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>19691</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="5143500"/>
+          <a:ext cx="4477375" cy="4591691"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>333953</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>19285</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="9763125"/>
+          <a:ext cx="4143953" cy="1686160"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing16.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>743692</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>9633</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="190500"/>
+          <a:ext cx="5315692" cy="771633"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>105428</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>152900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5334000" y="190500"/>
+          <a:ext cx="4677428" cy="3581900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>38637</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>9925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1333500"/>
+          <a:ext cx="3848637" cy="2867425"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2400,7 +3251,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -2481,7 +3332,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A58" workbookViewId="0">
       <selection activeCell="N51" sqref="N51"/>
     </sheetView>
   </sheetViews>
@@ -2496,7 +3347,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -2523,7 +3421,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -2570,7 +3468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
se relaizo y estilos a tarjetas seccion recomandado
</commit_message>
<xml_diff>
--- a/ANOTACIONES MOBILE DESIGN.xlsx
+++ b/ANOTACIONES MOBILE DESIGN.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="9" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="15" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="figma" sheetId="1" r:id="rId1"/>
@@ -29,6 +29,9 @@
     <sheet name="tarjetas secc beneficios" sheetId="16" r:id="rId15"/>
     <sheet name="comodin foto grande" sheetId="17" r:id="rId16"/>
     <sheet name="secc planes" sheetId="18" r:id="rId17"/>
+    <sheet name="tarjetas secc planes" sheetId="19" r:id="rId18"/>
+    <sheet name="estilo tarjetas" sheetId="20" r:id="rId19"/>
+    <sheet name="boton escoge este" sheetId="21" r:id="rId20"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -1784,6 +1787,325 @@
         <a:xfrm>
           <a:off x="0" y="1333500"/>
           <a:ext cx="3848637" cy="2867425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing17.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>724266</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>48412</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6486525" y="123825"/>
+          <a:ext cx="2619741" cy="5639587"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>286641</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>479</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="190500"/>
+          <a:ext cx="6382641" cy="3429479"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing18.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>753537</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>67163</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7611537" cy="3496163"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>162568</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>114632</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7743825" y="19050"/>
+          <a:ext cx="4610743" cy="2381582"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>257695</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>38495</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7962900" y="2543175"/>
+          <a:ext cx="3724795" cy="2829320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing19.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>448184</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>181665</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5181600" y="0"/>
+          <a:ext cx="3648584" cy="4944165"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>343226</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>171828</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4105275" y="5086350"/>
+          <a:ext cx="2333951" cy="2705478"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>543628</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>57594</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="76200" y="304800"/>
+          <a:ext cx="5039428" cy="3181794"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3392,13 +3714,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3414,6 +3767,20 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
termine la primera tarjeta de slide, voy a resolverr las 2 faltante yo solo
</commit_message>
<xml_diff>
--- a/ANOTACIONES MOBILE DESIGN.xlsx
+++ b/ANOTACIONES MOBILE DESIGN.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="15" activeTab="18"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="16" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="figma" sheetId="1" r:id="rId1"/>
@@ -32,6 +32,7 @@
     <sheet name="tarjetas secc planes" sheetId="19" r:id="rId18"/>
     <sheet name="estilo tarjetas" sheetId="20" r:id="rId19"/>
     <sheet name="boton escoge este" sheetId="21" r:id="rId20"/>
+    <sheet name="Hoja1" sheetId="22" r:id="rId21"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -2335,6 +2336,125 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing20.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>600903</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>171607</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="190500"/>
+          <a:ext cx="5934903" cy="1124107"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>705587</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>57716</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6096000" y="190500"/>
+          <a:ext cx="5277587" cy="4058216"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>695635</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>143001</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1714500"/>
+          <a:ext cx="2219635" cy="905001"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3729,7 +3849,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
@@ -3744,7 +3864,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
@@ -3775,8 +3895,21 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
terminado el proyeto con el css para tablets y pc
</commit_message>
<xml_diff>
--- a/ANOTACIONES MOBILE DESIGN.xlsx
+++ b/ANOTACIONES MOBILE DESIGN.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\eliezer\mobilefirst\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\eliezer\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="16" activeTab="17"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="18" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="figma" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,9 @@
     <sheet name="tarjetas secc planes" sheetId="19" r:id="rId18"/>
     <sheet name="estilo tarjetas" sheetId="20" r:id="rId19"/>
     <sheet name="boton escoge este" sheetId="21" r:id="rId20"/>
-    <sheet name="Hoja1" sheetId="22" r:id="rId21"/>
+    <sheet name="scroll" sheetId="22" r:id="rId21"/>
+    <sheet name="footer" sheetId="23" r:id="rId22"/>
+    <sheet name="media queries tablet" sheetId="24" r:id="rId23"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -2449,6 +2451,562 @@
         <a:xfrm>
           <a:off x="0" y="1714500"/>
           <a:ext cx="2219635" cy="905001"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing21.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>258047</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>95749</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4676775" y="1666875"/>
+          <a:ext cx="6249272" cy="3572374"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>343480</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>171793</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2095500"/>
+          <a:ext cx="4153480" cy="2457793"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>609601</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>695325</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Conector recto de flecha 6"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="2133601" y="2466975"/>
+          <a:ext cx="2371724" cy="276225"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>667869</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>162160</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagen 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="266700" y="0"/>
+          <a:ext cx="8021169" cy="1686160"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing22.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>19519</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>96026</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5800725" y="57150"/>
+          <a:ext cx="3362794" cy="5563376"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>343692</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>76503</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="190500"/>
+          <a:ext cx="5677692" cy="2172003"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>238584</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>114529</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2667000"/>
+          <a:ext cx="3286584" cy="1638529"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing23.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>152932</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>38287</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7772400" y="28575"/>
+          <a:ext cx="3810532" cy="1343212"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>200797</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>66760</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="28575"/>
+          <a:ext cx="5534797" cy="609685"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>267801</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>29080</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="981075"/>
+          <a:ext cx="7887801" cy="3620005"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>638689</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>152634</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="5524500"/>
+          <a:ext cx="3686689" cy="1676634"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>715645</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>585</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4572000" y="5524500"/>
+          <a:ext cx="9097645" cy="4191585"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>467322</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>213</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagen 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="10287000"/>
+          <a:ext cx="4277322" cy="1524213"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>734591</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>452</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagen 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4572000" y="10287000"/>
+          <a:ext cx="8354591" cy="3238952"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3849,7 +4407,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
@@ -3909,11 +4467,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
finalizado y porbado con lighthose el proyecto
</commit_message>
<xml_diff>
--- a/ANOTACIONES MOBILE DESIGN.xlsx
+++ b/ANOTACIONES MOBILE DESIGN.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\eliezer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\eliezer\mobilefirst\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="18" activeTab="22"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="19" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="figma" sheetId="1" r:id="rId1"/>
@@ -35,6 +35,7 @@
     <sheet name="scroll" sheetId="22" r:id="rId21"/>
     <sheet name="footer" sheetId="23" r:id="rId22"/>
     <sheet name="media queries tablet" sheetId="24" r:id="rId23"/>
+    <sheet name="medicion lighthouse" sheetId="25" r:id="rId24"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -3007,6 +3008,49 @@
         <a:xfrm>
           <a:off x="4572000" y="10287000"/>
           <a:ext cx="8354591" cy="3238952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing24.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>55524</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>75286</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="571500"/>
+          <a:ext cx="13009524" cy="7314286"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4497,8 +4541,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+    <sheetView topLeftCell="A61" workbookViewId="0">
       <selection activeCell="B76" sqref="B76"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>